<commit_message>
Deploying to gh-pages from  @ 152729cae9c6cc35cd560f78ea9d23814ee7ec01 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_6-2-2.xlsx
+++ b/assets/excel/2021_6-2-2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring_2021\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8943A44-ED4E-4519-8319-60F68801FA8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545EEBBD-C8E3-4BB9-9B86-5CF8DC2D9B81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{FA376DC0-5542-4490-8D9C-CE3D5F3816E5}"/>
   </bookViews>
@@ -1272,8 +1272,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:O332"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A301" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A325" sqref="A325:XFD325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10555,7 +10555,7 @@
     <row r="324" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C324" s="29"/>
     </row>
-    <row r="325" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C325" s="35" t="s">
         <v>90</v>
       </c>

</xml_diff>